<commit_message>
replacing names in templates to remove duplicates
</commit_message>
<xml_diff>
--- a/Projects/CCBZA/Data/Template_GROCERY_November.xlsx
+++ b/Projects/CCBZA/Data/Template_GROCERY_November.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="175">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">MERCHANDISING</t>
   </si>
   <si>
-    <t xml:space="preserve">Merchandising</t>
+    <t xml:space="preserve">Merchandise</t>
   </si>
   <si>
     <t xml:space="preserve">SOS, Price</t>
@@ -545,6 +545,9 @@
   </si>
   <si>
     <t xml:space="preserve">300ml Can Multipack, 1.5L 4 pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability SKU facing And</t>
   </si>
   <si>
     <t xml:space="preserve">Ambient Shelf</t>
@@ -754,7 +757,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -795,18 +798,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -828,14 +819,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -908,10 +891,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -988,6 +967,56 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>523440</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9943560" cy="9524520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
@@ -999,20 +1028,19 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.15348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="1020" min="8" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,7 +1089,7 @@
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1257,21 +1285,21 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" s="12" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11" t="s">
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="5" t="n">
@@ -1279,20 +1307,20 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11" t="s">
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="5" t="n">
@@ -1300,20 +1328,20 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11" t="s">
+      <c r="D15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="5" t="n">
@@ -1345,41 +1373,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="12" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1400,91 +1428,90 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q65536"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K4" activeCellId="0" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="72.3627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="114.693023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="118.260465116279"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.52093023255814"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.98139534883721"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="63.5023255813954"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.02790697674419"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.24651162790698"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="65.3441860465116"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -1493,402 +1520,400 @@
       <c r="C2" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19" t="n">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="L2" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="20"/>
+      <c r="L2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="16"/>
       <c r="O2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="P2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="19" t="n">
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="20"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="16"/>
       <c r="O3" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="25" t="n">
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="20"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="16"/>
       <c r="O4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="25" t="n">
-        <v>10</v>
-      </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="20"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="20" t="n">
+        <v>10</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="16"/>
       <c r="O5" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="26" t="n">
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="21" t="n">
         <v>15.5</v>
       </c>
-      <c r="K6" s="19" t="n">
+      <c r="K6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L6" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
+      <c r="L6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
       <c r="O6" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="26" t="n">
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="21" t="n">
         <v>15.5</v>
       </c>
-      <c r="K7" s="19" t="n">
+      <c r="K7" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
+      <c r="L7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="Q7" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="26" t="n">
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="21" t="n">
         <v>22</v>
       </c>
-      <c r="K8" s="19" t="n">
+      <c r="K8" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
+      <c r="L8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
       <c r="O8" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="26" t="n">
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="21" t="n">
         <v>22</v>
       </c>
-      <c r="K9" s="19" t="n">
+      <c r="K9" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L9" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
+      <c r="L9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P9" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="Q9" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="19" t="n">
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="K10" s="19" t="n">
+      <c r="K10" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L10" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
+      <c r="L10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
       <c r="O10" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P10" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="Q10" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="27" t="n">
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="K11" s="19" t="n">
+      <c r="K11" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L11" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
+      <c r="L11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
       <c r="O11" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P11" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q11" s="21" t="s">
+      <c r="Q11" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="19" t="n">
-        <v>10</v>
-      </c>
-      <c r="K12" s="19" t="n">
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="K12" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L12" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" s="20"/>
+      <c r="L12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" s="16"/>
       <c r="O12" s="0" t="s">
         <v>11</v>
       </c>
       <c r="P12" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="21" t="s">
+      <c r="Q12" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1897,7 +1922,8 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1913,244 +1939,243 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="48.6093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.1441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.02790697674419"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="50.0883720930233"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" s="12" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="15" t="n">
+      <c r="F2" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="29" t="s">
+      <c r="G2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" s="12" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="15" t="n">
+      <c r="F3" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="29"/>
+      <c r="G3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="21" t="n">
+      <c r="D4" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="19" t="n">
+      <c r="F4" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="21"/>
+      <c r="G4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="21" t="n">
+      <c r="D5" s="16" t="n">
         <v>27</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="19" t="n">
+      <c r="F5" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="21"/>
+      <c r="G5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="21" t="n">
+      <c r="D6" s="16" t="n">
         <v>19</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F6" s="19" t="n">
+      <c r="F6" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="21"/>
+      <c r="G6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="12" t="n">
+      <c r="D7" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F7" s="19" t="n">
+      <c r="F7" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="0" t="s">
         <v>91</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="19" t="n">
+      <c r="F8" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="0" t="s">
         <v>91</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>94</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="19" t="n">
+      <c r="F9" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2158,20 +2183,20 @@
       <c r="A10" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="0" t="s">
         <v>91</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="21" t="s">
+      <c r="F10" s="12"/>
+      <c r="G10" s="16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2179,20 +2204,20 @@
       <c r="A11" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="0" t="s">
         <v>91</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="21" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2216,156 +2241,155 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.1348837209302"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.98139534883721"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.0511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.7488372093023"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.24651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" s="20" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+    <row r="2" s="16" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="15" t="n">
+      <c r="H2" s="12" t="n">
         <v>75</v>
       </c>
-      <c r="N2" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" s="20" t="s">
+      <c r="N2" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="H3" s="15" t="n">
+      <c r="H3" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="N3" s="19" t="n">
+      <c r="N3" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="16" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="0" t="s">
@@ -2376,7 +2400,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -2385,25 +2409,25 @@
       <c r="C4" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H4" s="19" t="n">
+      <c r="H4" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="N4" s="19" t="n">
+      <c r="N4" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="R4" s="0" t="s">
@@ -2414,7 +2438,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -2423,25 +2447,25 @@
       <c r="C5" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H5" s="19" t="n">
+      <c r="H5" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="N5" s="19" t="n">
+      <c r="N5" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="16" t="s">
         <v>6</v>
       </c>
       <c r="R5" s="0" t="s">
@@ -2452,7 +2476,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -2461,25 +2485,25 @@
       <c r="C6" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="19" t="n">
+      <c r="H6" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="N6" s="19" t="n">
+      <c r="N6" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="16" t="s">
         <v>6</v>
       </c>
       <c r="R6" s="0" t="s">
@@ -2490,7 +2514,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -2499,25 +2523,25 @@
       <c r="C7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="19" t="n">
+      <c r="H7" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="N7" s="19" t="n">
+      <c r="N7" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="16" t="s">
         <v>6</v>
       </c>
       <c r="R7" s="0" t="s">
@@ -2528,7 +2552,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -2537,25 +2561,25 @@
       <c r="C8" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H8" s="19" t="n">
+      <c r="H8" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="N8" s="19" t="n">
+      <c r="N8" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="16" t="s">
         <v>6</v>
       </c>
       <c r="R8" s="0" t="s">
@@ -2590,69 +2614,68 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.98139534883721"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.24651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="30" t="s">
         <v>134</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="12" t="n">
         <v>4</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="20"/>
+      <c r="G2" s="16"/>
       <c r="I2" s="0" t="s">
         <v>10</v>
       </c>
@@ -2680,717 +2703,714 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.3627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="181.148837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.706976744186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.9302325581395"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.706976744186"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.7488372093023"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.553488372093"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="12.306976744186"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="103.618604651163"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="186.683720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="78.1441860465116"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.3674418604651"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="12.553488372093"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="106.693023255814"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="34.4558139534884"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" s="20" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+    <row r="2" s="16" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="K2" s="20" t="n">
+      <c r="K2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="15" t="n">
+      <c r="L2" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N2" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" s="21" t="s">
+      <c r="N2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="16" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="31" t="s">
         <v>142</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L3" s="15" t="n">
+      <c r="L3" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N3" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R3" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="21" t="s">
+      <c r="N3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="16" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="31" t="s">
         <v>144</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L4" s="15" t="n">
+      <c r="L4" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N4" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S4" s="21" t="s">
+      <c r="N4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="16" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="31" t="s">
         <v>146</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L5" s="15" t="n">
+      <c r="L5" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N5" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R5" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S5" s="21" t="s">
+      <c r="N5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="28" t="s">
         <v>148</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L6" s="15" t="n">
+      <c r="L6" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="M6" s="38" t="n">
+      <c r="M6" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="N6" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S6" s="21" t="s">
+      <c r="N6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="28" t="s">
         <v>150</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L7" s="15" t="n">
+      <c r="L7" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="M7" s="38" t="n">
-        <v>6</v>
-      </c>
-      <c r="N7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S7" s="21" t="s">
+      <c r="M7" s="33" t="n">
+        <v>6</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7" s="16" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="39" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="13" t="s">
         <v>154</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L8" s="15" t="n">
+      <c r="L8" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S8" s="21" t="s">
+      <c r="N8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="T8" s="15"/>
+      <c r="T8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="39" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="13" t="s">
         <v>154</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L9" s="15" t="n">
+      <c r="L9" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N9" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S9" s="21" t="s">
+      <c r="N9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S9" s="16" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" s="21" t="s">
+      <c r="C10" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="D10" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="33" t="s">
-        <v>159</v>
+      <c r="F10" s="28" t="s">
+        <v>160</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L10" s="15" t="n">
+      <c r="L10" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N10" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S10" s="21" t="s">
+      <c r="N10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" s="16" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="D11" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="26" t="s">
         <v>56</v>
       </c>
       <c r="J11" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="L11" s="15" t="n">
+      <c r="L11" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N11" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="R11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="S11" s="21" t="s">
+      <c r="N11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="S11" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>162</v>
-      </c>
       <c r="E12" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="F12" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="F12" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="16" t="s">
         <v>126</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="L12" s="15" t="n">
+        <v>168</v>
+      </c>
+      <c r="L12" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N12" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q12" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="R12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="S12" s="21" t="s">
+      <c r="N12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="S12" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>162</v>
-      </c>
       <c r="E13" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="G13" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="G13" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="26" t="s">
         <v>56</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="L13" s="15" t="n">
+      <c r="L13" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N13" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q13" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="R13" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="S13" s="21" t="s">
+      <c r="N13" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="S13" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="26" t="s">
         <v>56</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="L14" s="15" t="n">
+      <c r="L14" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N14" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q14" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="R14" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="S14" s="21" t="s">
+      <c r="N14" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="S14" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="26" t="s">
         <v>56</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="L15" s="15" t="n">
+      <c r="L15" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N15" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q15" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="R15" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="S15" s="21" t="s">
+      <c r="N15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R15" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="S15" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="16" t="s">
         <v>126</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="L16" s="15" t="n">
+        <v>174</v>
+      </c>
+      <c r="L16" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="N16" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q16" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="R16" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="S16" s="21" t="s">
-        <v>163</v>
+      <c r="N16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="S16" s="16" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>